<commit_message>
editing excel and profile
</commit_message>
<xml_diff>
--- a/src/main/metadata/documents/File/OnPremMigrationnPlan.xlsx
+++ b/src/main/metadata/documents/File/OnPremMigrationnPlan.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="78">
   <si>
     <t xml:space="preserve">Owner </t>
   </si>
@@ -257,6 +257,9 @@
   </si>
   <si>
     <t>Production job will be executed from Bamboo for 26th Major release</t>
+  </si>
+  <si>
+    <t>not started</t>
   </si>
 </sst>
 </file>
@@ -873,7 +876,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1118,7 +1121,9 @@
       <c r="E13" s="20">
         <v>43211</v>
       </c>
-      <c r="F13" s="1"/>
+      <c r="F13" s="1" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="14" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="1">

</xml_diff>